<commit_message>
Update with DoD %
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A75ED18-54E7-3041-8D1A-0941F0E6EA20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AC882A-11A0-BB4B-9653-136BB3BDF7D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" activeTab="1" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>确诊</t>
   </si>
@@ -98,19 +98,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1692,18 +1695,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:P8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1725,8 +1729,29 @@
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>43855</v>
       </c>
@@ -1748,8 +1773,35 @@
       <c r="H3" s="3">
         <v>56</v>
       </c>
+      <c r="J3" s="1">
+        <v>43855</v>
+      </c>
+      <c r="K3" s="4">
+        <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
+        <v>0.54181746397315256</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:P8" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
+        <v>0.54335218729863244</v>
+      </c>
+      <c r="M3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36590330788804071</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.53457653457653453</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36708860759493667</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36585365853658547</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>43854</v>
       </c>
@@ -1771,8 +1823,35 @@
       <c r="H4" s="3">
         <v>41</v>
       </c>
+      <c r="J4" s="1">
+        <v>43854</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K8" si="1">IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
+        <v>0.59850636373198696</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65878859857482186</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83302238805970141</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.55060240963855422</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33898305084745761</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.6399999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>43853</v>
       </c>
@@ -1794,8 +1873,35 @@
       <c r="H5" s="3">
         <v>25</v>
       </c>
+      <c r="J5" s="1">
+        <v>43853</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.61217568255044941</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.727735368956743</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45359019264448341</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.86315789473684212</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.47058823529411775</v>
+      </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>43852</v>
       </c>
@@ -1817,8 +1923,35 @@
       <c r="H6" s="3">
         <v>17</v>
       </c>
+      <c r="J6" s="1">
+        <v>43852</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6841147018661813</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="M6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>43851</v>
       </c>
@@ -1838,8 +1971,35 @@
       <c r="H7" s="3">
         <v>9</v>
       </c>
+      <c r="J7" s="1">
+        <v>43851</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="O7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>43850</v>
       </c>
@@ -1857,6 +2017,33 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="J8" s="1">
+        <v>43850</v>
+      </c>
+      <c r="K8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1867,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B86A94-8283-8644-87CD-E552D46DB91C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update for 1/26 data
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -2,13 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AC882A-11A0-BB4B-9653-136BB3BDF7D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D30A27B-077C-884B-9497-DC9D36637B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
@@ -259,26 +260,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$8</c:f>
+              <c:f>data!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -286,23 +290,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$3:$E$8</c:f>
+              <c:f>data!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>5794</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -343,26 +350,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$8</c:f>
+              <c:f>data!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -370,26 +380,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$3:$F$8</c:f>
+              <c:f>data!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>2744</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -430,26 +443,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$8</c:f>
+              <c:f>data!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -457,23 +473,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$3:$G$8</c:f>
+              <c:f>data!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -514,26 +533,29 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$8</c:f>
+              <c:f>data!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -541,23 +563,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$3:$H$8</c:f>
+              <c:f>data!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1365,10 +1390,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1695,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:P8"/>
+  <dimension ref="B2:P9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1753,295 +1778,346 @@
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C3" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D3" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E3" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F3" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G3" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H3" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="J3" s="1">
-        <v>43855</v>
+        <f>B3</f>
+        <v>43856</v>
       </c>
       <c r="K3" s="4">
         <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
-        <v>0.54181746397315256</v>
+        <v>0.39981221458751226</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:P8" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
-        <v>0.54335218729863244</v>
+        <f t="shared" ref="L3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
+        <v>0.41273891259974027</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36590330788804071</v>
+        <f t="shared" ref="M3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
+        <v>1.1587183308494784</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" si="0"/>
-        <v>0.53457653457653453</v>
+        <f t="shared" ref="N3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
+        <v>0.38936708860759484</v>
       </c>
       <c r="O3" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36708860759493667</v>
+        <f t="shared" ref="O3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
+        <v>0.42283950617283961</v>
       </c>
       <c r="P3" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36585365853658547</v>
+        <f t="shared" ref="P3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="C4" s="3">
-        <v>15197</v>
+        <v>23431</v>
       </c>
       <c r="D4" s="3">
-        <v>13967</v>
+        <v>21556</v>
       </c>
       <c r="E4" s="3">
-        <v>1965</v>
+        <v>2684</v>
       </c>
       <c r="F4" s="3">
-        <v>1287</v>
+        <v>1975</v>
       </c>
       <c r="G4" s="3">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="H4" s="3">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" ref="K4:K8" si="1">IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.59850636373198696</v>
+        <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
+        <v>0.54181746397315256</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.65878859857482186</v>
+        <f t="shared" ref="L4:P9" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
+        <v>0.54335218729863244</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.83302238805970141</v>
+        <f t="shared" si="5"/>
+        <v>0.36590330788804071</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.55060240963855422</v>
+        <f t="shared" si="5"/>
+        <v>0.53457653457653453</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.33898305084745761</v>
+        <f t="shared" si="5"/>
+        <v>0.36708860759493667</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.6399999999999999</v>
+        <f t="shared" si="5"/>
+        <v>0.36585365853658547</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="C5" s="3">
-        <v>9507</v>
+        <v>15197</v>
       </c>
       <c r="D5" s="3">
-        <v>8420</v>
+        <v>13967</v>
       </c>
       <c r="E5" s="3">
-        <v>1072</v>
+        <v>1965</v>
       </c>
       <c r="F5" s="3">
-        <v>830</v>
+        <v>1287</v>
       </c>
       <c r="G5" s="3">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="H5" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="J5" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="1"/>
-        <v>0.61217568255044941</v>
+        <f t="shared" ref="K5:K9" si="6">IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
+        <v>0.59850636373198696</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.70860389610389607</v>
+        <f t="shared" si="5"/>
+        <v>0.65878859857482186</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="0"/>
-        <v>1.727735368956743</v>
+        <f t="shared" si="5"/>
+        <v>0.83302238805970141</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.45359019264448341</v>
+        <f t="shared" si="5"/>
+        <v>0.55060240963855422</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.86315789473684212</v>
+        <f t="shared" si="5"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" si="0"/>
-        <v>0.47058823529411775</v>
+        <f t="shared" si="5"/>
+        <v>0.6399999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="C6" s="3">
-        <v>5897</v>
+        <v>9507</v>
       </c>
       <c r="D6" s="3">
-        <v>4928</v>
+        <v>8420</v>
       </c>
       <c r="E6" s="3">
-        <v>393</v>
+        <v>1072</v>
       </c>
       <c r="F6" s="3">
-        <v>571</v>
+        <v>830</v>
       </c>
       <c r="G6" s="3">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="H6" s="3">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J6" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="1"/>
-        <v>1.6841147018661813</v>
+        <f t="shared" si="6"/>
+        <v>0.61217568255044941</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="0"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="M6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="5"/>
+        <v>1.727735368956743</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.29772727272727262</v>
+        <f t="shared" si="5"/>
+        <v>0.45359019264448341</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="0"/>
-        <v>-6.8627450980392135E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.86315789473684212</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="5"/>
+        <v>0.47058823529411775</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="C7" s="3">
-        <v>2197</v>
+        <v>5897</v>
       </c>
       <c r="D7" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>4928</v>
+      </c>
+      <c r="E7" s="3">
+        <v>393</v>
+      </c>
       <c r="F7" s="3">
-        <v>440</v>
+        <v>571</v>
       </c>
       <c r="G7" s="3">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H7" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26336975273145491</v>
+        <f t="shared" si="6"/>
+        <v>1.6841147018661813</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="M7" s="4">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+        <f t="shared" si="5"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="M7" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="O7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
+        <v>43851</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2197</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1394</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>440</v>
+      </c>
+      <c r="G8" s="3">
+        <v>102</v>
+      </c>
+      <c r="H8" s="3">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1">
+        <v>43851</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="6"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="O8" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P8" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
         <v>43850</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>1739</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>922</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="3">
         <v>54</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="3">
         <v>291</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="J8" s="1">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="J9" s="1">
         <v>43850</v>
       </c>
-      <c r="K8" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="K9" s="4" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L8" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="L9" s="4" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="M8" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="M9" s="4" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="N8" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="N9" s="4" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="O8" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="O9" s="4" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="P8" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="P9" s="4" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2055,7 +2131,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Jan 27
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D30A27B-077C-884B-9497-DC9D36637B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B5B146-6100-A24E-A452-07F5590372CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" activeTab="1" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -260,29 +260,32 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$9</c:f>
+              <c:f>data!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -290,26 +293,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$3:$E$9</c:f>
+              <c:f>data!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6973</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -350,29 +356,32 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$9</c:f>
+              <c:f>data!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -380,29 +389,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$3:$F$9</c:f>
+              <c:f>data!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>4515</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -443,29 +455,32 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$9</c:f>
+              <c:f>data!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -473,26 +488,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$3:$G$9</c:f>
+              <c:f>data!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>976</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -533,29 +551,32 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$9</c:f>
+              <c:f>data!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -563,26 +584,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$3:$H$9</c:f>
+              <c:f>data!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1720,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:P9"/>
+  <dimension ref="B2:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1778,346 +1802,397 @@
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="C3" s="3">
-        <v>32799</v>
+        <v>47833</v>
       </c>
       <c r="D3" s="3">
-        <v>30453</v>
+        <v>44132</v>
       </c>
       <c r="E3" s="3">
-        <v>5794</v>
+        <v>6973</v>
       </c>
       <c r="F3" s="3">
-        <v>2744</v>
+        <v>4515</v>
       </c>
       <c r="G3" s="3">
-        <v>461</v>
+        <v>976</v>
       </c>
       <c r="H3" s="3">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="J3" s="1">
         <f>B3</f>
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="K3" s="4">
         <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
-        <v>0.39981221458751226</v>
+        <v>0.45836763315954765</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
-        <v>0.41273891259974027</v>
+        <v>0.44918398844120455</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
-        <v>1.1587183308494784</v>
+        <v>0.20348636520538488</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" ref="N3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
-        <v>0.38936708860759484</v>
+        <v>0.64540816326530615</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
-        <v>0.42283950617283961</v>
+        <v>1.1171366594360088</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" ref="P3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
-        <v>0.4285714285714286</v>
+        <v>0.32499999999999996</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C4" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D4" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E4" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F4" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G4" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H4" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="J4" s="1">
-        <v>43855</v>
+        <f>B4</f>
+        <v>43856</v>
       </c>
       <c r="K4" s="4">
         <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.54181746397315256</v>
+        <v>0.39981221458751226</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:P9" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.54335218729863244</v>
+        <f t="shared" ref="L4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
+        <v>0.41273891259974027</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="5"/>
-        <v>0.36590330788804071</v>
+        <f t="shared" ref="M4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
+        <v>1.1587183308494784</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="5"/>
-        <v>0.53457653457653453</v>
+        <f t="shared" ref="N4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
+        <v>0.38936708860759484</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" si="5"/>
-        <v>0.36708860759493667</v>
+        <f t="shared" ref="O4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
+        <v>0.42283950617283961</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" si="5"/>
-        <v>0.36585365853658547</v>
+        <f t="shared" ref="P4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="C5" s="3">
-        <v>15197</v>
+        <v>23431</v>
       </c>
       <c r="D5" s="3">
-        <v>13967</v>
+        <v>21556</v>
       </c>
       <c r="E5" s="3">
-        <v>1965</v>
+        <v>2684</v>
       </c>
       <c r="F5" s="3">
-        <v>1287</v>
+        <v>1975</v>
       </c>
       <c r="G5" s="3">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="H5" s="3">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="J5" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" ref="K5:K9" si="6">IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
-        <v>0.59850636373198696</v>
+        <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
+        <v>0.54181746397315256</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="5"/>
-        <v>0.65878859857482186</v>
+        <f t="shared" ref="L5:P10" si="10">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.54335218729863244</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="5"/>
-        <v>0.83302238805970141</v>
+        <f t="shared" si="10"/>
+        <v>0.36590330788804071</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="5"/>
-        <v>0.55060240963855422</v>
+        <f t="shared" si="10"/>
+        <v>0.53457653457653453</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="5"/>
-        <v>0.33898305084745761</v>
+        <f t="shared" si="10"/>
+        <v>0.36708860759493667</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" si="5"/>
-        <v>0.6399999999999999</v>
+        <f t="shared" si="10"/>
+        <v>0.36585365853658547</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="C6" s="3">
-        <v>9507</v>
+        <v>15197</v>
       </c>
       <c r="D6" s="3">
-        <v>8420</v>
+        <v>13967</v>
       </c>
       <c r="E6" s="3">
-        <v>1072</v>
+        <v>1965</v>
       </c>
       <c r="F6" s="3">
-        <v>830</v>
+        <v>1287</v>
       </c>
       <c r="G6" s="3">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="H6" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="J6" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="6"/>
-        <v>0.61217568255044941</v>
+        <f t="shared" ref="K6:K10" si="11">IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
+        <v>0.59850636373198696</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="5"/>
-        <v>0.70860389610389607</v>
+        <f t="shared" si="10"/>
+        <v>0.65878859857482186</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="5"/>
-        <v>1.727735368956743</v>
+        <f t="shared" si="10"/>
+        <v>0.83302238805970141</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="5"/>
-        <v>0.45359019264448341</v>
+        <f t="shared" si="10"/>
+        <v>0.55060240963855422</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="5"/>
-        <v>0.86315789473684212</v>
+        <f t="shared" si="10"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" si="5"/>
-        <v>0.47058823529411775</v>
+        <f t="shared" si="10"/>
+        <v>0.6399999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="C7" s="3">
-        <v>5897</v>
+        <v>9507</v>
       </c>
       <c r="D7" s="3">
-        <v>4928</v>
+        <v>8420</v>
       </c>
       <c r="E7" s="3">
-        <v>393</v>
+        <v>1072</v>
       </c>
       <c r="F7" s="3">
-        <v>571</v>
+        <v>830</v>
       </c>
       <c r="G7" s="3">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="H7" s="3">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J7" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="6"/>
-        <v>1.6841147018661813</v>
+        <f t="shared" si="11"/>
+        <v>0.61217568255044941</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="5"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="M7" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="10"/>
+        <v>1.727735368956743</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="5"/>
-        <v>0.29772727272727262</v>
+        <f t="shared" si="10"/>
+        <v>0.45359019264448341</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="5"/>
-        <v>-6.8627450980392135E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.86315789473684212</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" si="5"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="10"/>
+        <v>0.47058823529411775</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="C8" s="3">
-        <v>2197</v>
+        <v>5897</v>
       </c>
       <c r="D8" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>4928</v>
+      </c>
+      <c r="E8" s="3">
+        <v>393</v>
+      </c>
       <c r="F8" s="3">
-        <v>440</v>
+        <v>571</v>
       </c>
       <c r="G8" s="3">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H8" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J8" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="6"/>
-        <v>0.26336975273145491</v>
+        <f t="shared" si="11"/>
+        <v>1.6841147018661813</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="5"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="M8" s="4">
-        <f t="shared" si="5"/>
-        <v>-1</v>
+        <f t="shared" si="10"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="M8" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="5"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="O8" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P8" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="10"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="10"/>
+        <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
+        <v>43851</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2197</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1394</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>440</v>
+      </c>
+      <c r="G9" s="3">
+        <v>102</v>
+      </c>
+      <c r="H9" s="3">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>43851</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="11"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="10"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="10"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="O9" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="P9" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>43850</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>1739</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>922</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="3">
         <v>54</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>291</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="J9" s="1">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="J10" s="1">
         <v>43850</v>
       </c>
-      <c r="K9" s="4" t="str">
-        <f t="shared" si="6"/>
+      <c r="K10" s="4" t="str">
+        <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="L9" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="L10" s="4" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="M9" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="M10" s="4" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="N9" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="N10" s="4" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="O9" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="O10" s="4" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="P9" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="P10" s="4" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -2130,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B86A94-8283-8644-87CD-E552D46DB91C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Jan 28 data
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B5B146-6100-A24E-A452-07F5590372CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F777FF9-8886-0942-A3B0-BA3789601755}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2240" windowWidth="32200" windowHeight="25640" activeTab="1" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="10060" yWindow="460" windowWidth="34180" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>确诊</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>死亡率</t>
   </si>
 </sst>
 </file>
@@ -104,12 +107,13 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -260,32 +264,35 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$10</c:f>
+              <c:f>data!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -293,29 +300,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$3:$E$10</c:f>
+              <c:f>data!$E$3:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>9239</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6973</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -356,32 +366,35 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$10</c:f>
+              <c:f>data!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -389,32 +402,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$3:$F$10</c:f>
+              <c:f>data!$F$3:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>5974</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4515</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -455,32 +471,35 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$10</c:f>
+              <c:f>data!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -488,29 +507,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$3:$G$10</c:f>
+              <c:f>data!$G$3:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>1239</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>976</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -551,32 +573,35 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$10</c:f>
+              <c:f>data!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -584,29 +609,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$3:$H$10</c:f>
+              <c:f>data!$H$3:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1744,19 +1772,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:P10"/>
+  <dimension ref="B2:Q11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1799,400 +1830,482 @@
       <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="Q2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="C3" s="3">
-        <v>47833</v>
+        <v>65537</v>
       </c>
       <c r="D3" s="3">
-        <v>44132</v>
+        <v>59990</v>
       </c>
       <c r="E3" s="3">
-        <v>6973</v>
+        <v>9239</v>
       </c>
       <c r="F3" s="3">
-        <v>4515</v>
+        <v>5974</v>
       </c>
       <c r="G3" s="3">
-        <v>976</v>
+        <v>1239</v>
       </c>
       <c r="H3" s="3">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="J3" s="1">
         <f>B3</f>
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="K3" s="4">
         <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
-        <v>0.45836763315954765</v>
+        <v>0.37012104613969443</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
-        <v>0.44918398844120455</v>
+        <v>0.35933109761624227</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
-        <v>0.20348636520538488</v>
+        <v>0.32496773268320656</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" ref="N3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
-        <v>0.64540816326530615</v>
+        <v>0.32314507198228126</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
-        <v>1.1171366594360088</v>
+        <v>0.26946721311475419</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" ref="P3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
-        <v>0.32499999999999996</v>
+        <v>0.24528301886792447</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>H3/F3</f>
+        <v>2.2095748242383664E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="C4" s="3">
-        <v>32799</v>
+        <v>47833</v>
       </c>
       <c r="D4" s="3">
-        <v>30453</v>
+        <v>44132</v>
       </c>
       <c r="E4" s="3">
-        <v>5794</v>
+        <v>6973</v>
       </c>
       <c r="F4" s="3">
-        <v>2744</v>
+        <v>4515</v>
       </c>
       <c r="G4" s="3">
-        <v>461</v>
+        <v>976</v>
       </c>
       <c r="H4" s="3">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="J4" s="1">
         <f>B4</f>
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="K4" s="4">
         <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.39981221458751226</v>
+        <v>0.45836763315954765</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.41273891259974027</v>
+        <v>0.44918398844120455</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
-        <v>1.1587183308494784</v>
+        <v>0.20348636520538488</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" ref="N4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
-        <v>0.38936708860759484</v>
+        <v>0.64540816326530615</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" ref="O4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
-        <v>0.42283950617283961</v>
+        <v>1.1171366594360088</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
-        <v>0.4285714285714286</v>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" ref="Q4:Q9" si="10">H4/F4</f>
+        <v>2.3477297895902548E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C5" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D5" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E5" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F5" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G5" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H5" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="J5" s="1">
-        <v>43855</v>
+        <f>B5</f>
+        <v>43856</v>
       </c>
       <c r="K5" s="4">
         <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
+        <v>0.39981221458751226</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5" si="11">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.41273891259974027</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" ref="M5" si="12">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+        <v>1.1587183308494784</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ref="N5" si="13">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+        <v>0.38936708860759484</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" ref="O5" si="14">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+        <v>0.42283950617283961</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" ref="P5" si="15">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="10"/>
+        <v>2.9154518950437316E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>43855</v>
+      </c>
+      <c r="C6" s="3">
+        <v>23431</v>
+      </c>
+      <c r="D6" s="3">
+        <v>21556</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2684</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1975</v>
+      </c>
+      <c r="G6" s="3">
+        <v>324</v>
+      </c>
+      <c r="H6" s="3">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1">
+        <v>43855</v>
+      </c>
+      <c r="K6" s="4">
+        <f>IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
         <v>0.54181746397315256</v>
       </c>
-      <c r="L5" s="4">
-        <f t="shared" ref="L5:P10" si="10">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+      <c r="L6" s="4">
+        <f t="shared" ref="L6:P11" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
         <v>0.54335218729863244</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M6" s="4">
+        <f t="shared" si="16"/>
+        <v>0.36590330788804071</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="16"/>
+        <v>0.53457653457653453</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="16"/>
+        <v>0.36708860759493667</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="16"/>
+        <v>0.36585365853658547</v>
+      </c>
+      <c r="Q6" s="5">
         <f t="shared" si="10"/>
-        <v>0.36590330788804071</v>
-      </c>
-      <c r="N5" s="4">
+        <v>2.8354430379746835E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>43854</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15197</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13967</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1965</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1287</v>
+      </c>
+      <c r="G7" s="3">
+        <v>237</v>
+      </c>
+      <c r="H7" s="3">
+        <v>41</v>
+      </c>
+      <c r="J7" s="1">
+        <v>43854</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" ref="K7:K11" si="17">IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
+        <v>0.59850636373198696</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.65878859857482186</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.83302238805970141</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.55060240963855422</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.33898305084745761</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="Q7" s="5">
         <f t="shared" si="10"/>
-        <v>0.53457653457653453</v>
-      </c>
-      <c r="O5" s="4">
+        <v>3.1857031857031856E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>43853</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9507</v>
+      </c>
+      <c r="D8" s="3">
+        <v>8420</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1072</v>
+      </c>
+      <c r="F8" s="3">
+        <v>830</v>
+      </c>
+      <c r="G8" s="3">
+        <v>177</v>
+      </c>
+      <c r="H8" s="3">
+        <v>25</v>
+      </c>
+      <c r="J8" s="1">
+        <v>43853</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="17"/>
+        <v>0.61217568255044941</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="16"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="16"/>
+        <v>1.727735368956743</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="16"/>
+        <v>0.45359019264448341</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="16"/>
+        <v>0.86315789473684212</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="16"/>
+        <v>0.47058823529411775</v>
+      </c>
+      <c r="Q8" s="5">
         <f t="shared" si="10"/>
-        <v>0.36708860759493667</v>
-      </c>
-      <c r="P5" s="4">
+        <v>3.0120481927710843E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>43852</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5897</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4928</v>
+      </c>
+      <c r="E9" s="3">
+        <v>393</v>
+      </c>
+      <c r="F9" s="3">
+        <v>571</v>
+      </c>
+      <c r="G9" s="3">
+        <v>95</v>
+      </c>
+      <c r="H9" s="3">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1">
+        <v>43852</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="17"/>
+        <v>1.6841147018661813</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="16"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="M9" s="4" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="16"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="16"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="16"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="Q9" s="5">
         <f t="shared" si="10"/>
-        <v>0.36585365853658547</v>
+        <v>2.9772329246935202E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="1">
-        <v>43854</v>
-      </c>
-      <c r="C6" s="3">
-        <v>15197</v>
-      </c>
-      <c r="D6" s="3">
-        <v>13967</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1965</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1287</v>
-      </c>
-      <c r="G6" s="3">
-        <v>237</v>
-      </c>
-      <c r="H6" s="3">
-        <v>41</v>
-      </c>
-      <c r="J6" s="1">
-        <v>43854</v>
-      </c>
-      <c r="K6" s="4">
-        <f t="shared" ref="K6:K10" si="11">IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
-        <v>0.59850636373198696</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="10"/>
-        <v>0.65878859857482186</v>
-      </c>
-      <c r="M6" s="4">
-        <f t="shared" si="10"/>
-        <v>0.83302238805970141</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="10"/>
-        <v>0.55060240963855422</v>
-      </c>
-      <c r="O6" s="4">
-        <f t="shared" si="10"/>
-        <v>0.33898305084745761</v>
-      </c>
-      <c r="P6" s="4">
-        <f t="shared" si="10"/>
-        <v>0.6399999999999999</v>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>43851</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2197</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1394</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>440</v>
+      </c>
+      <c r="G10" s="3">
+        <v>102</v>
+      </c>
+      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1">
+        <v>43851</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="17"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="16"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="16"/>
+        <v>-1</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="16"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="O10" s="4" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="P10" s="4" t="str">
+        <f t="shared" si="16"/>
+        <v/>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1">
-        <v>43853</v>
-      </c>
-      <c r="C7" s="3">
-        <v>9507</v>
-      </c>
-      <c r="D7" s="3">
-        <v>8420</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1072</v>
-      </c>
-      <c r="F7" s="3">
-        <v>830</v>
-      </c>
-      <c r="G7" s="3">
-        <v>177</v>
-      </c>
-      <c r="H7" s="3">
-        <v>25</v>
-      </c>
-      <c r="J7" s="1">
-        <v>43853</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" si="11"/>
-        <v>0.61217568255044941</v>
-      </c>
-      <c r="L7" s="4">
-        <f t="shared" si="10"/>
-        <v>0.70860389610389607</v>
-      </c>
-      <c r="M7" s="4">
-        <f t="shared" si="10"/>
-        <v>1.727735368956743</v>
-      </c>
-      <c r="N7" s="4">
-        <f t="shared" si="10"/>
-        <v>0.45359019264448341</v>
-      </c>
-      <c r="O7" s="4">
-        <f t="shared" si="10"/>
-        <v>0.86315789473684212</v>
-      </c>
-      <c r="P7" s="4">
-        <f t="shared" si="10"/>
-        <v>0.47058823529411775</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="1">
-        <v>43852</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5897</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4928</v>
-      </c>
-      <c r="E8" s="3">
-        <v>393</v>
-      </c>
-      <c r="F8" s="3">
-        <v>571</v>
-      </c>
-      <c r="G8" s="3">
-        <v>95</v>
-      </c>
-      <c r="H8" s="3">
-        <v>17</v>
-      </c>
-      <c r="J8" s="1">
-        <v>43852</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="11"/>
-        <v>1.6841147018661813</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="10"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="M8" s="4" t="str">
-        <f t="shared" si="10"/>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>43850</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1739</v>
+      </c>
+      <c r="D11" s="3">
+        <v>922</v>
+      </c>
+      <c r="E11" s="3">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3">
+        <v>291</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="J11" s="1">
+        <v>43850</v>
+      </c>
+      <c r="K11" s="4" t="str">
+        <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="N8" s="4">
-        <f t="shared" si="10"/>
-        <v>0.29772727272727262</v>
-      </c>
-      <c r="O8" s="4">
-        <f t="shared" si="10"/>
-        <v>-6.8627450980392135E-2</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" si="10"/>
-        <v>0.88888888888888884</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
-        <v>43851</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2197</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <v>440</v>
-      </c>
-      <c r="G9" s="3">
-        <v>102</v>
-      </c>
-      <c r="H9" s="3">
-        <v>9</v>
-      </c>
-      <c r="J9" s="1">
-        <v>43851</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="11"/>
-        <v>0.26336975273145491</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="10"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="10"/>
-        <v>-1</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="10"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="O9" s="4" t="str">
-        <f t="shared" si="10"/>
+      <c r="L11" s="4" t="str">
+        <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="P9" s="4" t="str">
-        <f t="shared" si="10"/>
+      <c r="M11" s="4" t="str">
+        <f t="shared" si="16"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
-        <v>43850</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1739</v>
-      </c>
-      <c r="D10" s="3">
-        <v>922</v>
-      </c>
-      <c r="E10" s="3">
-        <v>54</v>
-      </c>
-      <c r="F10" s="3">
-        <v>291</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="J10" s="1">
-        <v>43850</v>
-      </c>
-      <c r="K10" s="4" t="str">
-        <f t="shared" si="11"/>
+      <c r="N11" s="4" t="str">
+        <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="L10" s="4" t="str">
-        <f t="shared" si="10"/>
+      <c r="O11" s="4" t="str">
+        <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="M10" s="4" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N10" s="4" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="O10" s="4" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="P10" s="4" t="str">
-        <f t="shared" si="10"/>
+      <c r="P11" s="4" t="str">
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -2205,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B86A94-8283-8644-87CD-E552D46DB91C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix broken URLs and add death rate
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F777FF9-8886-0942-A3B0-BA3789601755}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7E53E6-1A11-FF46-9E01-CD718FC3928E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="460" windowWidth="34180" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="25940" yWindow="1280" windowWidth="34180" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>确诊</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>死亡率</t>
+  </si>
+  <si>
+    <t>治愈</t>
   </si>
 </sst>
 </file>
@@ -226,9 +229,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.5050183833836636E-2"/>
-          <c:y val="8.3448769914647142E-2"/>
+          <c:y val="4.8068940654010343E-2"/>
           <c:w val="0.92375958218854382"/>
-          <c:h val="0.81843621802329147"/>
+          <c:h val="0.8538160708579482"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1444,8 +1447,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1772,22 +1775,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:Q11"/>
+  <dimension ref="B2:R11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" customWidth="1"/>
-    <col min="14" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1809,32 +1813,35 @@
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>43858</v>
       </c>
@@ -1856,40 +1863,43 @@
       <c r="H3" s="3">
         <v>132</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3" s="3">
+        <v>103</v>
+      </c>
+      <c r="K3" s="1">
         <f>B3</f>
         <v>43858</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
         <v>0.37012104613969443</v>
       </c>
-      <c r="L3" s="4">
-        <f t="shared" ref="L3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
+      <c r="M3" s="4">
+        <f t="shared" ref="M3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
         <v>0.35933109761624227</v>
       </c>
-      <c r="M3" s="4">
-        <f t="shared" ref="M3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
+      <c r="N3" s="4">
+        <f t="shared" ref="N3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
         <v>0.32496773268320656</v>
       </c>
-      <c r="N3" s="4">
-        <f t="shared" ref="N3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
         <v>0.32314507198228126</v>
       </c>
-      <c r="O3" s="4">
-        <f t="shared" ref="O3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
         <v>0.26946721311475419</v>
       </c>
-      <c r="P3" s="4">
-        <f t="shared" ref="P3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
         <v>0.24528301886792447</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
         <f>H3/F3</f>
         <v>2.2095748242383664E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>43857</v>
       </c>
@@ -1911,40 +1921,43 @@
       <c r="H4" s="3">
         <v>106</v>
       </c>
-      <c r="J4" s="1">
+      <c r="I4" s="3">
+        <v>60</v>
+      </c>
+      <c r="K4" s="1">
         <f>B4</f>
         <v>43857</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
         <v>0.45836763315954765</v>
       </c>
-      <c r="L4" s="4">
-        <f t="shared" ref="L4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
+      <c r="M4" s="4">
+        <f t="shared" ref="M4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
         <v>0.44918398844120455</v>
       </c>
-      <c r="M4" s="4">
-        <f t="shared" ref="M4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
         <v>0.20348636520538488</v>
       </c>
-      <c r="N4" s="4">
-        <f t="shared" ref="N4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
         <v>0.64540816326530615</v>
       </c>
-      <c r="O4" s="4">
-        <f t="shared" ref="O4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
+      <c r="P4" s="4">
+        <f t="shared" ref="P4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
         <v>1.1171366594360088</v>
       </c>
-      <c r="P4" s="4">
-        <f t="shared" ref="P4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
+      <c r="Q4" s="4">
+        <f t="shared" ref="Q4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
         <v>0.32499999999999996</v>
       </c>
-      <c r="Q4" s="5">
-        <f t="shared" ref="Q4:Q9" si="10">H4/F4</f>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:R9" si="10">H4/F4</f>
         <v>2.3477297895902548E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>43856</v>
       </c>
@@ -1966,40 +1979,43 @@
       <c r="H5" s="3">
         <v>80</v>
       </c>
-      <c r="J5" s="1">
+      <c r="I5" s="3">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1">
         <f>B5</f>
         <v>43856</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
         <v>0.39981221458751226</v>
       </c>
-      <c r="L5" s="4">
-        <f t="shared" ref="L5" si="11">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+      <c r="M5" s="4">
+        <f t="shared" ref="M5" si="11">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
         <v>0.41273891259974027</v>
       </c>
-      <c r="M5" s="4">
-        <f t="shared" ref="M5" si="12">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+      <c r="N5" s="4">
+        <f t="shared" ref="N5" si="12">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
         <v>1.1587183308494784</v>
       </c>
-      <c r="N5" s="4">
-        <f t="shared" ref="N5" si="13">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+      <c r="O5" s="4">
+        <f t="shared" ref="O5" si="13">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
         <v>0.38936708860759484</v>
       </c>
-      <c r="O5" s="4">
-        <f t="shared" ref="O5" si="14">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+      <c r="P5" s="4">
+        <f t="shared" ref="P5" si="14">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
         <v>0.42283950617283961</v>
       </c>
-      <c r="P5" s="4">
-        <f t="shared" ref="P5" si="15">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5" si="15">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
         <v>0.4285714285714286</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <f t="shared" si="10"/>
         <v>2.9154518950437316E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>43855</v>
       </c>
@@ -2021,39 +2037,42 @@
       <c r="H6" s="3">
         <v>56</v>
       </c>
-      <c r="J6" s="1">
+      <c r="I6" s="3">
+        <v>49</v>
+      </c>
+      <c r="K6" s="1">
         <v>43855</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <f>IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
         <v>0.54181746397315256</v>
       </c>
-      <c r="L6" s="4">
-        <f t="shared" ref="L6:P11" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
+      <c r="M6" s="4">
+        <f t="shared" ref="M6:Q11" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
         <v>0.54335218729863244</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <f t="shared" si="16"/>
         <v>0.36590330788804071</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f t="shared" si="16"/>
         <v>0.53457653457653453</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <f t="shared" si="16"/>
         <v>0.36708860759493667</v>
       </c>
-      <c r="P6" s="4">
+      <c r="Q6" s="4">
         <f t="shared" si="16"/>
         <v>0.36585365853658547</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <f t="shared" si="10"/>
         <v>2.8354430379746835E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>43854</v>
       </c>
@@ -2075,39 +2094,42 @@
       <c r="H7" s="3">
         <v>41</v>
       </c>
-      <c r="J7" s="1">
+      <c r="I7" s="3">
+        <v>38</v>
+      </c>
+      <c r="K7" s="1">
         <v>43854</v>
       </c>
-      <c r="K7" s="4">
-        <f t="shared" ref="K7:K11" si="17">IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
+      <c r="L7" s="4">
+        <f t="shared" ref="L7:L11" si="17">IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
         <v>0.59850636373198696</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <f t="shared" si="16"/>
         <v>0.65878859857482186</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <f t="shared" si="16"/>
         <v>0.83302238805970141</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="16"/>
         <v>0.55060240963855422</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <f t="shared" si="16"/>
         <v>0.33898305084745761</v>
       </c>
-      <c r="P7" s="4">
+      <c r="Q7" s="4">
         <f t="shared" si="16"/>
         <v>0.6399999999999999</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="5">
         <f t="shared" si="10"/>
         <v>3.1857031857031856E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>43853</v>
       </c>
@@ -2129,39 +2151,42 @@
       <c r="H8" s="3">
         <v>25</v>
       </c>
-      <c r="J8" s="1">
+      <c r="I8" s="3">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1">
         <v>43853</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <f t="shared" si="17"/>
         <v>0.61217568255044941</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <f t="shared" si="16"/>
         <v>0.70860389610389607</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <f t="shared" si="16"/>
         <v>1.727735368956743</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <f t="shared" si="16"/>
         <v>0.45359019264448341</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <f t="shared" si="16"/>
         <v>0.86315789473684212</v>
       </c>
-      <c r="P8" s="4">
+      <c r="Q8" s="4">
         <f t="shared" si="16"/>
         <v>0.47058823529411775</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <f t="shared" si="10"/>
         <v>3.0120481927710843E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>43852</v>
       </c>
@@ -2183,39 +2208,40 @@
       <c r="H9" s="3">
         <v>17</v>
       </c>
-      <c r="J9" s="1">
+      <c r="I9" s="3"/>
+      <c r="K9" s="1">
         <v>43852</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <f t="shared" si="17"/>
         <v>1.6841147018661813</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <f t="shared" si="16"/>
         <v>2.5351506456241033</v>
       </c>
-      <c r="M9" s="4" t="str">
+      <c r="N9" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <f t="shared" si="16"/>
         <v>0.29772727272727262</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <f t="shared" si="16"/>
         <v>-6.8627450980392135E-2</v>
       </c>
-      <c r="P9" s="4">
+      <c r="Q9" s="4">
         <f t="shared" si="16"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <f t="shared" si="10"/>
         <v>2.9772329246935202E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>43851</v>
       </c>
@@ -2235,35 +2261,36 @@
       <c r="H10" s="3">
         <v>9</v>
       </c>
-      <c r="J10" s="1">
+      <c r="I10" s="3"/>
+      <c r="K10" s="1">
         <v>43851</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <f t="shared" si="17"/>
         <v>0.26336975273145491</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <f t="shared" si="16"/>
         <v>0.51193058568329719</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <f t="shared" si="16"/>
         <v>-1</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <f t="shared" si="16"/>
         <v>0.51202749140893467</v>
       </c>
-      <c r="O10" s="4" t="str">
+      <c r="P10" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="P10" s="4" t="str">
+      <c r="Q10" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>43850</v>
       </c>
@@ -2281,30 +2308,31 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="J11" s="1">
+      <c r="I11" s="3"/>
+      <c r="K11" s="1">
         <v>43850</v>
       </c>
-      <c r="K11" s="4" t="str">
+      <c r="L11" s="4" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="L11" s="4" t="str">
+      <c r="M11" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="M11" s="4" t="str">
+      <c r="N11" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="N11" s="4" t="str">
+      <c r="O11" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="O11" s="4" t="str">
+      <c r="P11" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="P11" s="4" t="str">
+      <c r="Q11" s="4" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
@@ -2319,7 +2347,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Jan 29 data
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7E53E6-1A11-FF46-9E01-CD718FC3928E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6C02F0-9FBA-E145-BF22-B966AADD39EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25940" yWindow="1280" windowWidth="34180" windowHeight="25640" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="34560" yWindow="1000" windowWidth="34180" windowHeight="11240" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -110,13 +110,14 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -267,35 +268,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$11</c:f>
+              <c:f>data!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -303,32 +307,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$3:$E$11</c:f>
+              <c:f>data!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>12167</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9239</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6973</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -369,35 +376,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$11</c:f>
+              <c:f>data!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -405,35 +415,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$3:$F$11</c:f>
+              <c:f>data!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>7711</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5974</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4515</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -474,35 +487,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$11</c:f>
+              <c:f>data!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -510,32 +526,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$3:$G$11</c:f>
+              <c:f>data!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1239</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>976</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -576,35 +595,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$11</c:f>
+              <c:f>data!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -612,32 +634,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$3:$H$11</c:f>
+              <c:f>data!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1775,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:R11"/>
+  <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1843,499 +1868,569 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="C3" s="3">
-        <v>65537</v>
+        <v>88693</v>
       </c>
       <c r="D3" s="3">
-        <v>59990</v>
+        <v>81947</v>
       </c>
       <c r="E3" s="3">
-        <v>9239</v>
+        <v>12167</v>
       </c>
       <c r="F3" s="3">
-        <v>5974</v>
+        <v>7711</v>
       </c>
       <c r="G3" s="3">
-        <v>1239</v>
+        <v>1370</v>
       </c>
       <c r="H3" s="3">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="I3" s="3">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K3" s="1">
         <f>B3</f>
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="L3" s="4">
         <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
-        <v>0.37012104613969443</v>
+        <v>0.35332712818713086</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
-        <v>0.35933109761624227</v>
+        <v>0.36601100183363888</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" ref="N3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
-        <v>0.32496773268320656</v>
+        <v>0.31691741530468676</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
-        <v>0.32314507198228126</v>
+        <v>0.2907599598259123</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" ref="P3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
-        <v>0.26946721311475419</v>
+        <v>0.10573042776432606</v>
       </c>
       <c r="Q3" s="4">
         <f t="shared" ref="Q3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
-        <v>0.24528301886792447</v>
+        <v>0.28787878787878785</v>
       </c>
       <c r="R3" s="5">
         <f>H3/F3</f>
-        <v>2.2095748242383664E-2</v>
+        <v>2.2046427181947867E-2</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="C4" s="3">
-        <v>47833</v>
+        <v>65537</v>
       </c>
       <c r="D4" s="3">
-        <v>44132</v>
+        <v>59990</v>
       </c>
       <c r="E4" s="3">
-        <v>6973</v>
+        <v>9239</v>
       </c>
       <c r="F4" s="3">
-        <v>4515</v>
+        <v>5974</v>
       </c>
       <c r="G4" s="3">
-        <v>976</v>
+        <v>1239</v>
       </c>
       <c r="H4" s="3">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="I4" s="3">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="K4" s="1">
         <f>B4</f>
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="L4" s="4">
         <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.45836763315954765</v>
+        <v>0.37012104613969443</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.44918398844120455</v>
+        <v>0.35933109761624227</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" ref="N4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
-        <v>0.20348636520538488</v>
+        <v>0.32496773268320656</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" ref="O4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
-        <v>0.64540816326530615</v>
+        <v>0.32314507198228126</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
-        <v>1.1171366594360088</v>
+        <v>0.26946721311475419</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
-        <v>0.32499999999999996</v>
+        <v>0.24528301886792447</v>
       </c>
       <c r="R4" s="5">
-        <f t="shared" ref="R4:R9" si="10">H4/F4</f>
-        <v>2.3477297895902548E-2</v>
+        <f>H4/F4</f>
+        <v>2.2095748242383664E-2</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="C5" s="3">
-        <v>32799</v>
+        <v>47833</v>
       </c>
       <c r="D5" s="3">
-        <v>30453</v>
+        <v>44132</v>
       </c>
       <c r="E5" s="3">
-        <v>5794</v>
+        <v>6973</v>
       </c>
       <c r="F5" s="3">
-        <v>2744</v>
+        <v>4515</v>
       </c>
       <c r="G5" s="3">
-        <v>461</v>
+        <v>976</v>
       </c>
       <c r="H5" s="3">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="I5" s="3">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="K5" s="1">
         <f>B5</f>
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="L5" s="4">
         <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
-        <v>0.39981221458751226</v>
+        <v>0.45836763315954765</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5" si="11">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
-        <v>0.41273891259974027</v>
+        <f t="shared" ref="M5" si="10">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.44918398844120455</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" ref="N5" si="12">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
-        <v>1.1587183308494784</v>
+        <f t="shared" ref="N5" si="11">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+        <v>0.20348636520538488</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O5" si="13">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
-        <v>0.38936708860759484</v>
+        <f t="shared" ref="O5" si="12">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+        <v>0.64540816326530615</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" ref="P5" si="14">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
-        <v>0.42283950617283961</v>
+        <f t="shared" ref="P5" si="13">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+        <v>1.1171366594360088</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5" si="15">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
-        <v>0.4285714285714286</v>
+        <f t="shared" ref="Q5" si="14">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+        <v>0.32499999999999996</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" si="10"/>
-        <v>2.9154518950437316E-2</v>
+        <f t="shared" ref="R5:R10" si="15">H5/F5</f>
+        <v>2.3477297895902548E-2</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C6" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D6" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E6" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F6" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G6" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H6" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="I6" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K6" s="1">
-        <v>43855</v>
+        <f>B6</f>
+        <v>43856</v>
       </c>
       <c r="L6" s="4">
         <f>IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
-        <v>0.54181746397315256</v>
+        <v>0.39981221458751226</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6:Q11" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
-        <v>0.54335218729863244</v>
+        <f t="shared" ref="M6" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
+        <v>0.41273891259974027</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="16"/>
-        <v>0.36590330788804071</v>
+        <f t="shared" ref="N6" si="17">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
+        <v>1.1587183308494784</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="16"/>
-        <v>0.53457653457653453</v>
+        <f t="shared" ref="O6" si="18">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
+        <v>0.38936708860759484</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" si="16"/>
-        <v>0.36708860759493667</v>
+        <f t="shared" ref="P6" si="19">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
+        <v>0.42283950617283961</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="16"/>
-        <v>0.36585365853658547</v>
+        <f t="shared" ref="Q6" si="20">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
+        <v>0.4285714285714286</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" si="10"/>
-        <v>2.8354430379746835E-2</v>
+        <f t="shared" si="15"/>
+        <v>2.9154518950437316E-2</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="C7" s="3">
-        <v>15197</v>
+        <v>23431</v>
       </c>
       <c r="D7" s="3">
-        <v>13967</v>
+        <v>21556</v>
       </c>
       <c r="E7" s="3">
-        <v>1965</v>
+        <v>2684</v>
       </c>
       <c r="F7" s="3">
-        <v>1287</v>
+        <v>1975</v>
       </c>
       <c r="G7" s="3">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="H7" s="3">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I7" s="3">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K7" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L11" si="17">IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
-        <v>0.59850636373198696</v>
+        <f>IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
+        <v>0.54181746397315256</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="16"/>
-        <v>0.65878859857482186</v>
+        <f t="shared" ref="M7:Q12" si="21">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
+        <v>0.54335218729863244</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="16"/>
-        <v>0.83302238805970141</v>
+        <f t="shared" si="21"/>
+        <v>0.36590330788804071</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="16"/>
-        <v>0.55060240963855422</v>
+        <f t="shared" si="21"/>
+        <v>0.53457653457653453</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" si="16"/>
-        <v>0.33898305084745761</v>
+        <f t="shared" si="21"/>
+        <v>0.36708860759493667</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="16"/>
-        <v>0.6399999999999999</v>
+        <f t="shared" si="21"/>
+        <v>0.36585365853658547</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" si="10"/>
-        <v>3.1857031857031856E-2</v>
+        <f t="shared" si="15"/>
+        <v>2.8354430379746835E-2</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="C8" s="3">
-        <v>9507</v>
+        <v>15197</v>
       </c>
       <c r="D8" s="3">
-        <v>8420</v>
+        <v>13967</v>
       </c>
       <c r="E8" s="3">
-        <v>1072</v>
+        <v>1965</v>
       </c>
       <c r="F8" s="3">
-        <v>830</v>
+        <v>1287</v>
       </c>
       <c r="G8" s="3">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="H8" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I8" s="3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K8" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="17"/>
-        <v>0.61217568255044941</v>
+        <f t="shared" ref="L8:L12" si="22">IF(ISERROR(C8/C9-1)=TRUE, "", C8/C9-1)</f>
+        <v>0.59850636373198696</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="16"/>
-        <v>0.70860389610389607</v>
+        <f t="shared" si="21"/>
+        <v>0.65878859857482186</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="16"/>
-        <v>1.727735368956743</v>
+        <f t="shared" si="21"/>
+        <v>0.83302238805970141</v>
       </c>
       <c r="O8" s="4">
-        <f t="shared" si="16"/>
-        <v>0.45359019264448341</v>
+        <f t="shared" si="21"/>
+        <v>0.55060240963855422</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" si="16"/>
-        <v>0.86315789473684212</v>
+        <f t="shared" si="21"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="16"/>
-        <v>0.47058823529411775</v>
+        <f t="shared" si="21"/>
+        <v>0.6399999999999999</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="10"/>
-        <v>3.0120481927710843E-2</v>
+        <f t="shared" si="15"/>
+        <v>3.1857031857031856E-2</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="C9" s="3">
-        <v>5897</v>
+        <v>9507</v>
       </c>
       <c r="D9" s="3">
-        <v>4928</v>
+        <v>8420</v>
       </c>
       <c r="E9" s="3">
-        <v>393</v>
+        <v>1072</v>
       </c>
       <c r="F9" s="3">
-        <v>571</v>
+        <v>830</v>
       </c>
       <c r="G9" s="3">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="H9" s="3">
-        <v>17</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="I9" s="3">
+        <v>34</v>
+      </c>
       <c r="K9" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="17"/>
-        <v>1.6841147018661813</v>
+        <f t="shared" si="22"/>
+        <v>0.61217568255044941</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="16"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="N9" s="4" t="str">
-        <f t="shared" si="16"/>
-        <v/>
+        <f t="shared" si="21"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="21"/>
+        <v>1.727735368956743</v>
       </c>
       <c r="O9" s="4">
-        <f t="shared" si="16"/>
-        <v>0.29772727272727262</v>
+        <f t="shared" si="21"/>
+        <v>0.45359019264448341</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" si="16"/>
-        <v>-6.8627450980392135E-2</v>
+        <f t="shared" si="21"/>
+        <v>0.86315789473684212</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="16"/>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="21"/>
+        <v>0.47058823529411775</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="10"/>
-        <v>2.9772329246935202E-2</v>
+        <f t="shared" si="15"/>
+        <v>3.0120481927710843E-2</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="C10" s="3">
-        <v>2197</v>
+        <v>5897</v>
       </c>
       <c r="D10" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>4928</v>
+      </c>
+      <c r="E10" s="3">
+        <v>393</v>
+      </c>
       <c r="F10" s="3">
-        <v>440</v>
+        <v>571</v>
       </c>
       <c r="G10" s="3">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H10" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I10" s="3"/>
       <c r="K10" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="17"/>
-        <v>0.26336975273145491</v>
+        <f t="shared" si="22"/>
+        <v>1.6841147018661813</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="16"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="N10" s="4">
-        <f t="shared" si="16"/>
-        <v>-1</v>
+        <f t="shared" si="21"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="N10" s="4" t="str">
+        <f t="shared" si="21"/>
+        <v/>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="16"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="P10" s="4" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="Q10" s="4" t="str">
-        <f t="shared" si="16"/>
-        <v/>
+        <f t="shared" si="21"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="21"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="21"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="15"/>
+        <v>2.9772329246935202E-2</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
-        <v>43850</v>
+        <v>43851</v>
       </c>
       <c r="C11" s="3">
-        <v>1739</v>
+        <v>2197</v>
       </c>
       <c r="D11" s="3">
-        <v>922</v>
-      </c>
-      <c r="E11" s="3">
-        <v>54</v>
-      </c>
+        <v>1394</v>
+      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="3">
-        <v>291</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+        <v>440</v>
+      </c>
+      <c r="G11" s="3">
+        <v>102</v>
+      </c>
+      <c r="H11" s="3">
+        <v>9</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="K11" s="1">
+        <v>43851</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="22"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="21"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="21"/>
+        <v>-1</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="21"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="P11" s="4" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="Q11" s="4" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>43850</v>
       </c>
-      <c r="L11" s="4" t="str">
-        <f t="shared" si="17"/>
+      <c r="C12" s="3">
+        <v>1739</v>
+      </c>
+      <c r="D12" s="3">
+        <v>922</v>
+      </c>
+      <c r="E12" s="3">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3">
+        <v>291</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="1">
+        <v>43850</v>
+      </c>
+      <c r="L12" s="4" t="str">
+        <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="M11" s="4" t="str">
-        <f t="shared" si="16"/>
+      <c r="M12" s="4" t="str">
+        <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="N11" s="4" t="str">
-        <f t="shared" si="16"/>
+      <c r="N12" s="4" t="str">
+        <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="O11" s="4" t="str">
-        <f t="shared" si="16"/>
+      <c r="O12" s="4" t="str">
+        <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="P11" s="4" t="str">
-        <f t="shared" si="16"/>
+      <c r="P12" s="4" t="str">
+        <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="Q11" s="4" t="str">
-        <f t="shared" si="16"/>
+      <c r="Q12" s="4" t="str">
+        <f t="shared" si="21"/>
         <v/>
       </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2347,7 +2442,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Jan 30 and add 2 more charts
</commit_message>
<xml_diff>
--- a/pandemic2020.xlsx
+++ b/pandemic2020.xlsx
@@ -9,13 +9,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6C02F0-9FBA-E145-BF22-B966AADD39EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43E856-74A7-7E47-895B-DC33807DC050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="1000" windowWidth="34180" windowHeight="11240" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="6320" yWindow="460" windowWidth="31160" windowHeight="24140" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="chart" sheetId="2" r:id="rId2"/>
+    <sheet name="chart-LTD" sheetId="2" r:id="rId2"/>
+    <sheet name="chart-Net New Daily" sheetId="3" r:id="rId3"/>
+    <sheet name="chart-LTD-Death-Cured" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>确诊</t>
   </si>
@@ -54,6 +56,15 @@
   </si>
   <si>
     <t>治愈</t>
+  </si>
+  <si>
+    <t>Life-To-Date</t>
+  </si>
+  <si>
+    <t>Life-To-Date DoD%</t>
+  </si>
+  <si>
+    <t>Daily Net New</t>
   </si>
 </sst>
 </file>
@@ -88,12 +99,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,7 +139,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -118,6 +147,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -126,6 +163,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF37D279"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -183,7 +225,21 @@
                 <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>年新型冠状病毒感染趋势图</a:t>
+              <a:t>年新型冠状病毒感染趋势图 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> 累计数据</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1800" b="1">
               <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
@@ -230,9 +286,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.5050183833836636E-2"/>
-          <c:y val="4.8068940654010343E-2"/>
-          <c:w val="0.92375958218854382"/>
-          <c:h val="0.8538160708579482"/>
+          <c:y val="7.5846714013689448E-2"/>
+          <c:w val="0.8320662133142448"/>
+          <c:h val="0.83735898821470844"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -243,7 +299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$E$2</c:f>
+              <c:f>data!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -255,9 +311,7 @@
           <c:spPr>
             <a:ln w="76200" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -268,38 +322,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$12</c:f>
+              <c:f>data!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -307,35 +364,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$3:$E$12</c:f>
+              <c:f>data!$E$4:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>15238</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12167</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9239</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6973</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -353,7 +413,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$F$2</c:f>
+              <c:f>data!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -376,38 +436,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$12</c:f>
+              <c:f>data!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -415,38 +478,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$3:$F$12</c:f>
+              <c:f>data!$F$4:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>9692</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7711</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5974</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4515</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -464,7 +530,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$G$2</c:f>
+              <c:f>data!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -487,38 +553,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$12</c:f>
+              <c:f>data!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -526,35 +595,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$3:$G$12</c:f>
+              <c:f>data!$G$4:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1527</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1370</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1239</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>976</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -572,7 +644,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$H$2</c:f>
+              <c:f>data!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -595,38 +667,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$3:$B$12</c:f>
+              <c:f>data!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -634,35 +709,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$3:$H$12</c:f>
+              <c:f>data!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -716,7 +794,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -775,7 +853,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -808,8 +886,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12929806714140388"/>
-          <c:y val="0.11216933419869951"/>
+          <c:x val="0.16907077666428061"/>
+          <c:y val="8.5754271282127467E-2"/>
           <c:w val="0.18290946083418108"/>
           <c:h val="0.29996130343738137"/>
         </c:manualLayout>
@@ -838,7 +916,1353 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>2020</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>年新型冠状病毒感染趋势图 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> 每日新增</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5050183833836636E-2"/>
+          <c:y val="6.9345593257471291E-2"/>
+          <c:w val="0.87163332140300642"/>
+          <c:h val="0.85354317821565262"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$X$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>疑似病例</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$U$4:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$X$4:$X$12</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>393</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B33B-D74F-9D8B-92673D9D5EE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$Y$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>确诊</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$U$4:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Y$4:$Y$12</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1771</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>131</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B33B-D74F-9D8B-92673D9D5EE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$Z$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>重症病例</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$U$4:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$4:$Z$12</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B33B-D74F-9D8B-92673D9D5EE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$AA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>死亡</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$U$4:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AA$4:$AA$12</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B33B-D74F-9D8B-92673D9D5EE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1693198303"/>
+        <c:axId val="1515999807"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1693198303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515999807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1515999807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693198303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15202532211882605"/>
+          <c:y val="6.4370623483385334E-2"/>
+          <c:w val="0.16977272727272724"/>
+          <c:h val="0.40847065814886346"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>2020</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>年新型冠状病毒感染趋势图 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> 累计 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1">
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> 死亡和治愈</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9866589119541873E-2"/>
+          <c:y val="8.0122855164277099E-2"/>
+          <c:w val="0.89649704724409451"/>
+          <c:h val="0.84314268126907588"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>死亡</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$H$4:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C4E6-5B42-9B83-0FC85AA01D1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>治愈</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="76200" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43852</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43851</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$I$4:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C4E6-5B42-9B83-0FC85AA01D1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1693198303"/>
+        <c:axId val="1515999807"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1693198303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515999807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1515999807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Amazon Ember" panose="020B0603020204020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693198303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1133889584824624"/>
+          <c:y val="6.8144208389045696E-2"/>
+          <c:w val="0.10772727272727275"/>
+          <c:h val="0.23996751349477541"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -944,7 +2368,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1472,8 +4008,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1481,6 +4017,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E6878FA-B394-7747-834F-F0511574C7CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08867733-0C86-7C46-9D3C-62AC53ABDB04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A8111C-7F06-E448-98B2-AD1AD79BDA3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,637 +4422,1135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B2:R17"/>
+  <dimension ref="B1:AB25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.6640625" customWidth="1"/>
     <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.1640625" customWidth="1"/>
+    <col min="19" max="19" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="U3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="1">
-        <v>43859</v>
-      </c>
-      <c r="C3" s="3">
-        <v>88693</v>
-      </c>
-      <c r="D3" s="3">
-        <v>81947</v>
-      </c>
-      <c r="E3" s="3">
-        <v>12167</v>
-      </c>
-      <c r="F3" s="3">
-        <v>7711</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1370</v>
-      </c>
-      <c r="H3" s="3">
-        <v>170</v>
-      </c>
-      <c r="I3" s="3">
-        <v>124</v>
-      </c>
-      <c r="K3" s="1">
-        <f>B3</f>
-        <v>43859</v>
-      </c>
-      <c r="L3" s="4">
-        <f>IF(ISERROR(C3/C4-1)=TRUE, "", C3/C4-1)</f>
-        <v>0.35332712818713086</v>
-      </c>
-      <c r="M3" s="4">
-        <f t="shared" ref="M3" si="0">IF(ISERROR(D3/D4-1)=TRUE, "", D3/D4-1)</f>
-        <v>0.36601100183363888</v>
-      </c>
-      <c r="N3" s="4">
-        <f t="shared" ref="N3" si="1">IF(ISERROR(E3/E4-1)=TRUE, "", E3/E4-1)</f>
-        <v>0.31691741530468676</v>
-      </c>
-      <c r="O3" s="4">
-        <f t="shared" ref="O3" si="2">IF(ISERROR(F3/F4-1)=TRUE, "", F3/F4-1)</f>
-        <v>0.2907599598259123</v>
-      </c>
-      <c r="P3" s="4">
-        <f t="shared" ref="P3" si="3">IF(ISERROR(G3/G4-1)=TRUE, "", G3/G4-1)</f>
-        <v>0.10573042776432606</v>
-      </c>
-      <c r="Q3" s="4">
-        <f t="shared" ref="Q3" si="4">IF(ISERROR(H3/H4-1)=TRUE, "", H3/H4-1)</f>
-        <v>0.28787878787878785</v>
-      </c>
-      <c r="R3" s="5">
-        <f>H3/F3</f>
-        <v>2.2046427181947867E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="C4" s="3">
-        <v>65537</v>
+        <v>113579</v>
       </c>
       <c r="D4" s="3">
-        <v>59990</v>
+        <v>102427</v>
       </c>
       <c r="E4" s="3">
-        <v>9239</v>
+        <v>15238</v>
       </c>
       <c r="F4" s="3">
-        <v>5974</v>
+        <v>9692</v>
       </c>
       <c r="G4" s="3">
-        <v>1239</v>
+        <v>1527</v>
       </c>
       <c r="H4" s="3">
-        <v>132</v>
+        <v>213</v>
       </c>
       <c r="I4" s="3">
-        <v>103</v>
+        <v>171</v>
       </c>
       <c r="K4" s="1">
         <f>B4</f>
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="L4" s="4">
         <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.37012104613969443</v>
+        <v>0.28058584104720774</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" ref="M4" si="5">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.35933109761624227</v>
+        <f t="shared" ref="M4" si="0">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
+        <v>0.24991762968748099</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" ref="N4" si="6">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
-        <v>0.32496773268320656</v>
+        <f t="shared" ref="N4" si="1">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
+        <v>0.25240404372482939</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4" si="7">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
-        <v>0.32314507198228126</v>
+        <f t="shared" ref="O4" si="2">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
+        <v>0.25690571910258075</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" ref="P4" si="8">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
-        <v>0.26946721311475419</v>
+        <f t="shared" ref="P4" si="3">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
+        <v>0.11459854014598547</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4" si="9">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
-        <v>0.24528301886792447</v>
-      </c>
-      <c r="R4" s="5">
+        <f t="shared" ref="Q4:R4" si="4">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
+        <v>0.25294117647058822</v>
+      </c>
+      <c r="R4" s="4">
+        <f t="shared" si="4"/>
+        <v>0.37903225806451624</v>
+      </c>
+      <c r="S4" s="5">
         <f>H4/F4</f>
-        <v>2.2095748242383664E-2</v>
+        <v>2.1976888155179529E-2</v>
+      </c>
+      <c r="U4" s="1">
+        <f>K4</f>
+        <v>43860</v>
+      </c>
+      <c r="V4" s="14">
+        <f>C4-C5</f>
+        <v>24886</v>
+      </c>
+      <c r="W4" s="14">
+        <f t="shared" ref="W4:AB4" si="5">D4-D5</f>
+        <v>20480</v>
+      </c>
+      <c r="X4" s="14">
+        <f t="shared" si="5"/>
+        <v>3071</v>
+      </c>
+      <c r="Y4" s="14">
+        <f t="shared" si="5"/>
+        <v>1981</v>
+      </c>
+      <c r="Z4" s="14">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+      <c r="AA4" s="14">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="AB4" s="14">
+        <f t="shared" si="5"/>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43857</v>
+        <v>43859</v>
       </c>
       <c r="C5" s="3">
-        <v>47833</v>
+        <v>88693</v>
       </c>
       <c r="D5" s="3">
-        <v>44132</v>
+        <v>81947</v>
       </c>
       <c r="E5" s="3">
-        <v>6973</v>
+        <v>12167</v>
       </c>
       <c r="F5" s="3">
-        <v>4515</v>
+        <v>7711</v>
       </c>
       <c r="G5" s="3">
-        <v>976</v>
+        <v>1370</v>
       </c>
       <c r="H5" s="3">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="I5" s="3">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="K5" s="1">
         <f>B5</f>
-        <v>43857</v>
+        <v>43859</v>
       </c>
       <c r="L5" s="4">
         <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
-        <v>0.45836763315954765</v>
+        <v>0.35332712818713086</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5" si="10">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
-        <v>0.44918398844120455</v>
+        <f t="shared" ref="M5" si="6">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.36601100183363888</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" ref="N5" si="11">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
-        <v>0.20348636520538488</v>
+        <f t="shared" ref="N5" si="7">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+        <v>0.31691741530468676</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O5" si="12">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
-        <v>0.64540816326530615</v>
+        <f t="shared" ref="O5" si="8">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+        <v>0.2907599598259123</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" ref="P5" si="13">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
-        <v>1.1171366594360088</v>
+        <f t="shared" ref="P5" si="9">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+        <v>0.10573042776432606</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5" si="14">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="R5" s="5">
-        <f t="shared" ref="R5:R10" si="15">H5/F5</f>
-        <v>2.3477297895902548E-2</v>
+        <f t="shared" ref="Q5:R5" si="10">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+        <v>0.28787878787878785</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" si="10"/>
+        <v>0.20388349514563098</v>
+      </c>
+      <c r="S5" s="5">
+        <f>H5/F5</f>
+        <v>2.2046427181947867E-2</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:U14" si="11">K5</f>
+        <v>43859</v>
+      </c>
+      <c r="V5" s="14">
+        <f t="shared" ref="V5:V12" si="12">C5-C6</f>
+        <v>23156</v>
+      </c>
+      <c r="W5" s="14">
+        <f t="shared" ref="W5:W12" si="13">D5-D6</f>
+        <v>21957</v>
+      </c>
+      <c r="X5" s="14">
+        <f t="shared" ref="X5:X12" si="14">E5-E6</f>
+        <v>2928</v>
+      </c>
+      <c r="Y5" s="14">
+        <f t="shared" ref="Y5:Y12" si="15">F5-F6</f>
+        <v>1737</v>
+      </c>
+      <c r="Z5" s="14">
+        <f t="shared" ref="Z5:Z12" si="16">G5-G6</f>
+        <v>131</v>
+      </c>
+      <c r="AA5" s="14">
+        <f t="shared" ref="AA5:AA12" si="17">H5-H6</f>
+        <v>38</v>
+      </c>
+      <c r="AB5" s="14">
+        <f t="shared" ref="AB5:AB12" si="18">I5-I6</f>
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43856</v>
+        <v>43858</v>
       </c>
       <c r="C6" s="3">
-        <v>32799</v>
+        <v>65537</v>
       </c>
       <c r="D6" s="3">
-        <v>30453</v>
+        <v>59990</v>
       </c>
       <c r="E6" s="3">
-        <v>5794</v>
+        <v>9239</v>
       </c>
       <c r="F6" s="3">
-        <v>2744</v>
+        <v>5974</v>
       </c>
       <c r="G6" s="3">
-        <v>461</v>
+        <v>1239</v>
       </c>
       <c r="H6" s="3">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="I6" s="3">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="K6" s="1">
         <f>B6</f>
-        <v>43856</v>
+        <v>43858</v>
       </c>
       <c r="L6" s="4">
         <f>IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
-        <v>0.39981221458751226</v>
+        <v>0.37012104613969443</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6" si="16">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
-        <v>0.41273891259974027</v>
+        <f t="shared" ref="M6" si="19">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
+        <v>0.35933109761624227</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6" si="17">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
-        <v>1.1587183308494784</v>
+        <f t="shared" ref="N6" si="20">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
+        <v>0.32496773268320656</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" ref="O6" si="18">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
-        <v>0.38936708860759484</v>
+        <f t="shared" ref="O6" si="21">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
+        <v>0.32314507198228126</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" ref="P6" si="19">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
-        <v>0.42283950617283961</v>
+        <f t="shared" ref="P6" si="22">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
+        <v>0.26946721311475419</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" ref="Q6" si="20">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
-        <v>0.4285714285714286</v>
-      </c>
-      <c r="R6" s="5">
+        <f t="shared" ref="Q6:R6" si="23">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
+        <v>0.24528301886792447</v>
+      </c>
+      <c r="R6" s="4">
+        <f t="shared" si="23"/>
+        <v>0.71666666666666656</v>
+      </c>
+      <c r="S6" s="5">
+        <f>H6/F6</f>
+        <v>2.2095748242383664E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="11"/>
+        <v>43858</v>
+      </c>
+      <c r="V6" s="14">
+        <f t="shared" si="12"/>
+        <v>17704</v>
+      </c>
+      <c r="W6" s="14">
+        <f t="shared" si="13"/>
+        <v>15858</v>
+      </c>
+      <c r="X6" s="14">
+        <f t="shared" si="14"/>
+        <v>2266</v>
+      </c>
+      <c r="Y6" s="14">
         <f t="shared" si="15"/>
-        <v>2.9154518950437316E-2</v>
+        <v>1459</v>
+      </c>
+      <c r="Z6" s="14">
+        <f t="shared" si="16"/>
+        <v>263</v>
+      </c>
+      <c r="AA6" s="14">
+        <f t="shared" si="17"/>
+        <v>26</v>
+      </c>
+      <c r="AB6" s="14">
+        <f t="shared" si="18"/>
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43855</v>
+        <v>43857</v>
       </c>
       <c r="C7" s="3">
-        <v>23431</v>
+        <v>47833</v>
       </c>
       <c r="D7" s="3">
-        <v>21556</v>
+        <v>44132</v>
       </c>
       <c r="E7" s="3">
-        <v>2684</v>
+        <v>6973</v>
       </c>
       <c r="F7" s="3">
-        <v>1975</v>
+        <v>4515</v>
       </c>
       <c r="G7" s="3">
-        <v>324</v>
+        <v>976</v>
       </c>
       <c r="H7" s="3">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="I7" s="3">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="K7" s="1">
-        <v>43855</v>
+        <f>B7</f>
+        <v>43857</v>
       </c>
       <c r="L7" s="4">
         <f>IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
+        <v>0.45836763315954765</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" ref="M7" si="24">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
+        <v>0.44918398844120455</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" ref="N7" si="25">IF(ISERROR(E7/E8-1)=TRUE, "", E7/E8-1)</f>
+        <v>0.20348636520538488</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" ref="O7" si="26">IF(ISERROR(F7/F8-1)=TRUE, "", F7/F8-1)</f>
+        <v>0.64540816326530615</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" ref="P7" si="27">IF(ISERROR(G7/G8-1)=TRUE, "", G7/G8-1)</f>
+        <v>1.1171366594360088</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" ref="Q7:R7" si="28">IF(ISERROR(H7/H8-1)=TRUE, "", H7/H8-1)</f>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="R7" s="4">
+        <f t="shared" si="28"/>
+        <v>0.17647058823529416</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" ref="S7:S12" si="29">H7/F7</f>
+        <v>2.3477297895902548E-2</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="11"/>
+        <v>43857</v>
+      </c>
+      <c r="V7" s="14">
+        <f t="shared" si="12"/>
+        <v>15034</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="13"/>
+        <v>13679</v>
+      </c>
+      <c r="X7" s="14">
+        <f t="shared" si="14"/>
+        <v>1179</v>
+      </c>
+      <c r="Y7" s="14">
+        <f t="shared" si="15"/>
+        <v>1771</v>
+      </c>
+      <c r="Z7" s="14">
+        <f t="shared" si="16"/>
+        <v>515</v>
+      </c>
+      <c r="AA7" s="14">
+        <f t="shared" si="17"/>
+        <v>26</v>
+      </c>
+      <c r="AB7" s="14">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>43856</v>
+      </c>
+      <c r="C8" s="3">
+        <v>32799</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30453</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5794</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2744</v>
+      </c>
+      <c r="G8" s="3">
+        <v>461</v>
+      </c>
+      <c r="H8" s="3">
+        <v>80</v>
+      </c>
+      <c r="I8" s="3">
+        <v>51</v>
+      </c>
+      <c r="K8" s="1">
+        <f>B8</f>
+        <v>43856</v>
+      </c>
+      <c r="L8" s="4">
+        <f>IF(ISERROR(C8/C9-1)=TRUE, "", C8/C9-1)</f>
+        <v>0.39981221458751226</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" ref="M8" si="30">IF(ISERROR(D8/D9-1)=TRUE, "", D8/D9-1)</f>
+        <v>0.41273891259974027</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" ref="N8" si="31">IF(ISERROR(E8/E9-1)=TRUE, "", E8/E9-1)</f>
+        <v>1.1587183308494784</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" ref="O8" si="32">IF(ISERROR(F8/F9-1)=TRUE, "", F8/F9-1)</f>
+        <v>0.38936708860759484</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" ref="P8" si="33">IF(ISERROR(G8/G9-1)=TRUE, "", G8/G9-1)</f>
+        <v>0.42283950617283961</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" ref="Q8:R8" si="34">IF(ISERROR(H8/H9-1)=TRUE, "", H8/H9-1)</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="R8" s="4">
+        <f t="shared" si="34"/>
+        <v>4.081632653061229E-2</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="29"/>
+        <v>2.9154518950437316E-2</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="11"/>
+        <v>43856</v>
+      </c>
+      <c r="V8" s="14">
+        <f t="shared" si="12"/>
+        <v>9368</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="13"/>
+        <v>8897</v>
+      </c>
+      <c r="X8" s="14">
+        <f t="shared" si="14"/>
+        <v>3110</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="shared" si="15"/>
+        <v>769</v>
+      </c>
+      <c r="Z8" s="14">
+        <f t="shared" si="16"/>
+        <v>137</v>
+      </c>
+      <c r="AA8" s="14">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="AB8" s="14">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>43855</v>
+      </c>
+      <c r="C9" s="3">
+        <v>23431</v>
+      </c>
+      <c r="D9" s="3">
+        <v>21556</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2684</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1975</v>
+      </c>
+      <c r="G9" s="3">
+        <v>324</v>
+      </c>
+      <c r="H9" s="3">
+        <v>56</v>
+      </c>
+      <c r="I9" s="3">
+        <v>49</v>
+      </c>
+      <c r="K9" s="1">
+        <v>43855</v>
+      </c>
+      <c r="L9" s="4">
+        <f>IF(ISERROR(C9/C10-1)=TRUE, "", C9/C10-1)</f>
         <v>0.54181746397315256</v>
       </c>
-      <c r="M7" s="4">
-        <f t="shared" ref="M7:Q12" si="21">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
+      <c r="M9" s="4">
+        <f t="shared" ref="M9:R14" si="35">IF(ISERROR(D9/D10-1)=TRUE, "", D9/D10-1)</f>
         <v>0.54335218729863244</v>
       </c>
-      <c r="N7" s="4">
-        <f t="shared" si="21"/>
+      <c r="N9" s="4">
+        <f t="shared" si="35"/>
         <v>0.36590330788804071</v>
       </c>
-      <c r="O7" s="4">
-        <f t="shared" si="21"/>
+      <c r="O9" s="4">
+        <f t="shared" si="35"/>
         <v>0.53457653457653453</v>
       </c>
-      <c r="P7" s="4">
-        <f t="shared" si="21"/>
+      <c r="P9" s="4">
+        <f t="shared" si="35"/>
         <v>0.36708860759493667</v>
       </c>
-      <c r="Q7" s="4">
-        <f t="shared" si="21"/>
+      <c r="Q9" s="4">
+        <f t="shared" si="35"/>
         <v>0.36585365853658547</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R9" s="4">
+        <f t="shared" si="35"/>
+        <v>0.28947368421052633</v>
+      </c>
+      <c r="S9" s="5">
+        <f t="shared" si="29"/>
+        <v>2.8354430379746835E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="11"/>
+        <v>43855</v>
+      </c>
+      <c r="V9" s="14">
+        <f t="shared" si="12"/>
+        <v>8234</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" si="13"/>
+        <v>7589</v>
+      </c>
+      <c r="X9" s="14">
+        <f t="shared" si="14"/>
+        <v>719</v>
+      </c>
+      <c r="Y9" s="14">
         <f t="shared" si="15"/>
-        <v>2.8354430379746835E-2</v>
+        <v>688</v>
+      </c>
+      <c r="Z9" s="14">
+        <f t="shared" si="16"/>
+        <v>87</v>
+      </c>
+      <c r="AA9" s="14">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="AB9" s="14">
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="1">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>43854</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="3">
         <v>15197</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D10" s="3">
         <v>13967</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
         <v>1965</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F10" s="3">
         <v>1287</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G10" s="3">
         <v>237</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H10" s="3">
         <v>41</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I10" s="3">
         <v>38</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K10" s="1">
         <v>43854</v>
       </c>
-      <c r="L8" s="4">
-        <f t="shared" ref="L8:L12" si="22">IF(ISERROR(C8/C9-1)=TRUE, "", C8/C9-1)</f>
+      <c r="L10" s="4">
+        <f t="shared" ref="L10:L14" si="36">IF(ISERROR(C10/C11-1)=TRUE, "", C10/C11-1)</f>
         <v>0.59850636373198696</v>
       </c>
-      <c r="M8" s="4">
-        <f t="shared" si="21"/>
+      <c r="M10" s="4">
+        <f t="shared" si="35"/>
         <v>0.65878859857482186</v>
       </c>
-      <c r="N8" s="4">
-        <f t="shared" si="21"/>
+      <c r="N10" s="4">
+        <f t="shared" si="35"/>
         <v>0.83302238805970141</v>
       </c>
-      <c r="O8" s="4">
-        <f t="shared" si="21"/>
+      <c r="O10" s="4">
+        <f t="shared" si="35"/>
         <v>0.55060240963855422</v>
       </c>
-      <c r="P8" s="4">
-        <f t="shared" si="21"/>
+      <c r="P10" s="4">
+        <f t="shared" si="35"/>
         <v>0.33898305084745761</v>
       </c>
-      <c r="Q8" s="4">
-        <f t="shared" si="21"/>
+      <c r="Q10" s="4">
+        <f t="shared" si="35"/>
         <v>0.6399999999999999</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R10" s="4">
+        <f t="shared" si="35"/>
+        <v>0.11764705882352944</v>
+      </c>
+      <c r="S10" s="5">
+        <f t="shared" si="29"/>
+        <v>3.1857031857031856E-2</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="11"/>
+        <v>43854</v>
+      </c>
+      <c r="V10" s="14">
+        <f t="shared" si="12"/>
+        <v>5690</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="13"/>
+        <v>5547</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="14"/>
+        <v>893</v>
+      </c>
+      <c r="Y10" s="14">
         <f t="shared" si="15"/>
-        <v>3.1857031857031856E-2</v>
+        <v>457</v>
+      </c>
+      <c r="Z10" s="14">
+        <f t="shared" si="16"/>
+        <v>60</v>
+      </c>
+      <c r="AA10" s="14">
+        <f t="shared" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="AB10" s="14">
+        <f t="shared" si="18"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>43853</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C11" s="3">
         <v>9507</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D11" s="3">
         <v>8420</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E11" s="3">
         <v>1072</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F11" s="3">
         <v>830</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G11" s="3">
         <v>177</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H11" s="3">
         <v>25</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I11" s="3">
         <v>34</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K11" s="1">
         <v>43853</v>
       </c>
-      <c r="L9" s="4">
-        <f t="shared" si="22"/>
+      <c r="L11" s="4">
+        <f t="shared" si="36"/>
         <v>0.61217568255044941</v>
       </c>
-      <c r="M9" s="4">
-        <f t="shared" si="21"/>
+      <c r="M11" s="4">
+        <f t="shared" si="35"/>
         <v>0.70860389610389607</v>
       </c>
-      <c r="N9" s="4">
-        <f t="shared" si="21"/>
+      <c r="N11" s="4">
+        <f t="shared" si="35"/>
         <v>1.727735368956743</v>
       </c>
-      <c r="O9" s="4">
-        <f t="shared" si="21"/>
+      <c r="O11" s="4">
+        <f t="shared" si="35"/>
         <v>0.45359019264448341</v>
       </c>
-      <c r="P9" s="4">
-        <f t="shared" si="21"/>
+      <c r="P11" s="4">
+        <f t="shared" si="35"/>
         <v>0.86315789473684212</v>
       </c>
-      <c r="Q9" s="4">
-        <f t="shared" si="21"/>
+      <c r="Q11" s="4">
+        <f t="shared" si="35"/>
         <v>0.47058823529411775</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R11" s="4" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="S11" s="5">
+        <f t="shared" si="29"/>
+        <v>3.0120481927710843E-2</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="11"/>
+        <v>43853</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="12"/>
+        <v>3610</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="13"/>
+        <v>3492</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="14"/>
+        <v>679</v>
+      </c>
+      <c r="Y11" s="14">
         <f t="shared" si="15"/>
-        <v>3.0120481927710843E-2</v>
+        <v>259</v>
+      </c>
+      <c r="Z11" s="14">
+        <f t="shared" si="16"/>
+        <v>82</v>
+      </c>
+      <c r="AA11" s="14">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="AB11" s="14">
+        <f t="shared" si="18"/>
+        <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>43852</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C12" s="3">
         <v>5897</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D12" s="3">
         <v>4928</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E12" s="3">
         <v>393</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F12" s="3">
         <v>571</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G12" s="3">
         <v>95</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H12" s="3">
         <v>17</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="K10" s="1">
-        <v>43852</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="22"/>
-        <v>1.6841147018661813</v>
-      </c>
-      <c r="M10" s="4">
-        <f t="shared" si="21"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="N10" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="O10" s="4">
-        <f t="shared" si="21"/>
-        <v>0.29772727272727262</v>
-      </c>
-      <c r="P10" s="4">
-        <f t="shared" si="21"/>
-        <v>-6.8627450980392135E-2</v>
-      </c>
-      <c r="Q10" s="4">
-        <f t="shared" si="21"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="R10" s="5">
-        <f t="shared" si="15"/>
-        <v>2.9772329246935202E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
-        <v>43851</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2197</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <v>440</v>
-      </c>
-      <c r="G11" s="3">
-        <v>102</v>
-      </c>
-      <c r="H11" s="3">
-        <v>9</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="K11" s="1">
-        <v>43851</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="22"/>
-        <v>0.26336975273145491</v>
-      </c>
-      <c r="M11" s="4">
-        <f t="shared" si="21"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="N11" s="4">
-        <f t="shared" si="21"/>
-        <v>-1</v>
-      </c>
-      <c r="O11" s="4">
-        <f t="shared" si="21"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="P11" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="Q11" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="1">
-        <v>43850</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1739</v>
-      </c>
-      <c r="D12" s="3">
-        <v>922</v>
-      </c>
-      <c r="E12" s="3">
-        <v>54</v>
-      </c>
-      <c r="F12" s="3">
-        <v>291</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="K12" s="1">
+        <v>43852</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="36"/>
+        <v>1.6841147018661813</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="35"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="N12" s="4" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="35"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="35"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="35"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" s="5">
+        <f t="shared" si="29"/>
+        <v>2.9772329246935202E-2</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="11"/>
+        <v>43852</v>
+      </c>
+      <c r="V12" s="14">
+        <f t="shared" si="12"/>
+        <v>3700</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" si="13"/>
+        <v>3534</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" si="14"/>
+        <v>393</v>
+      </c>
+      <c r="Y12" s="14">
+        <f t="shared" si="15"/>
+        <v>131</v>
+      </c>
+      <c r="Z12" s="14">
+        <f t="shared" si="16"/>
+        <v>-7</v>
+      </c>
+      <c r="AA12" s="14">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="AB12" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>43851</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2197</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1394</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>440</v>
+      </c>
+      <c r="G13" s="3">
+        <v>102</v>
+      </c>
+      <c r="H13" s="3">
+        <v>9</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="K13" s="1">
+        <v>43851</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="36"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="35"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="35"/>
+        <v>-1</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="35"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="P13" s="4" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="Q13" s="4" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R13" s="4"/>
+      <c r="U13" s="1">
+        <f t="shared" si="11"/>
+        <v>43851</v>
+      </c>
+      <c r="V13" s="4" t="str">
+        <f t="shared" ref="V13:V14" si="37">IF(ISERROR(M13/M14-1)=TRUE, "", M13/M14-1)</f>
+        <v/>
+      </c>
+      <c r="W13" s="4" t="str">
+        <f t="shared" ref="W13:W14" si="38">IF(ISERROR(N13/N14-1)=TRUE, "", N13/N14-1)</f>
+        <v/>
+      </c>
+      <c r="X13" s="4" t="str">
+        <f t="shared" ref="X13:X14" si="39">IF(ISERROR(O13/O14-1)=TRUE, "", O13/O14-1)</f>
+        <v/>
+      </c>
+      <c r="Y13" s="4" t="str">
+        <f t="shared" ref="Y13:Y14" si="40">IF(ISERROR(P13/P14-1)=TRUE, "", P13/P14-1)</f>
+        <v/>
+      </c>
+      <c r="Z13" s="4" t="str">
+        <f t="shared" ref="Z13:Z14" si="41">IF(ISERROR(Q13/Q14-1)=TRUE, "", Q13/Q14-1)</f>
+        <v/>
+      </c>
+      <c r="AA13" s="4" t="str">
+        <f t="shared" ref="AA13:AA14" si="42">IF(ISERROR(R13/R14-1)=TRUE, "", R13/R14-1)</f>
+        <v/>
+      </c>
+      <c r="AB13" s="4"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
         <v>43850</v>
       </c>
-      <c r="L12" s="4" t="str">
-        <f t="shared" si="22"/>
+      <c r="C14" s="3">
+        <v>1739</v>
+      </c>
+      <c r="D14" s="3">
+        <v>922</v>
+      </c>
+      <c r="E14" s="3">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3">
+        <v>291</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="1">
+        <v>43850</v>
+      </c>
+      <c r="L14" s="4" t="str">
+        <f t="shared" si="36"/>
         <v/>
       </c>
-      <c r="M12" s="4" t="str">
-        <f t="shared" si="21"/>
+      <c r="M14" s="4" t="str">
+        <f t="shared" si="35"/>
         <v/>
       </c>
-      <c r="N12" s="4" t="str">
-        <f t="shared" si="21"/>
+      <c r="N14" s="4" t="str">
+        <f t="shared" si="35"/>
         <v/>
       </c>
-      <c r="O12" s="4" t="str">
-        <f t="shared" si="21"/>
+      <c r="O14" s="4" t="str">
+        <f t="shared" si="35"/>
         <v/>
       </c>
-      <c r="P12" s="4" t="str">
-        <f t="shared" si="21"/>
+      <c r="P14" s="4" t="str">
+        <f t="shared" si="35"/>
         <v/>
       </c>
-      <c r="Q12" s="4" t="str">
-        <f t="shared" si="21"/>
+      <c r="Q14" s="4" t="str">
+        <f t="shared" si="35"/>
         <v/>
       </c>
+      <c r="R14" s="4"/>
+      <c r="U14" s="1">
+        <f t="shared" si="11"/>
+        <v>43850</v>
+      </c>
+      <c r="V14" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="W14" s="4" t="str">
+        <f t="shared" si="38"/>
+        <v/>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="Y14" s="4" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="Z14" s="4" t="str">
+        <f t="shared" si="41"/>
+        <v/>
+      </c>
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="42"/>
+        <v/>
+      </c>
+      <c r="AB14" s="4"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2442,7 +5562,37 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="I46" sqref="I46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB18AA0-2B3E-A04D-B5CB-2E1022114C46}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673EE37A-1131-9E4A-AD70-5B0BD03BB53B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>